<commit_message>
Crear/Actualizar Excel para pedido 69134d11b9c1d30b15fabdc3
</commit_message>
<xml_diff>
--- a/TEST_DEFINITIVO.xlsx
+++ b/TEST_DEFINITIVO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,10 +532,6 @@
           <t>1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>Inversor híbrido monofásico SUN-6k-SG05LP1-EU</t>
@@ -556,16 +552,65 @@
           <t>1</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
           <t>2024-01-03T10:49:29.104Z</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2488</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Test Ringover (NO TOCAR)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Estructura coplanar NOVOTEGRA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Inversor híbrido monofásico SUN-6k-SG05LP1-EU</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>BATERÍA LITIO SIGEN ENERGY SIGENSTOR 8,0KW</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>2024-01-03T10:49:29.104Z</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Crear/Actualizar Excel para pedido 6903661db7cb420aeabeeab5
</commit_message>
<xml_diff>
--- a/TEST_DEFINITIVO.xlsx
+++ b/TEST_DEFINITIVO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1017,7 +1017,6 @@
           <t>Estructura coplanar NOVOTEGRA</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
           <t>1</t>
@@ -1066,6 +1065,64 @@
       <c r="N12" t="inlineStr">
         <is>
           <t>2024-01-03T10:49:29.104Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2187</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Samuel Rupérez Macarro</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Estructura coplanar NOVOTEGRA</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>MODULO FV JA SOLAR 535WP BLACK FRAME BIFACIAL 120 CELDAS</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>GOODWE ES UNIQ - GW8000-ES-C10 híbrido monofásico</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>GOODWE Batería Lynx Home U G3 5,12 kWh</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>2025-09-25T07:50:43.054Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Crear/Actualizar Excel para pedido 691b59eb90ee710b08f4ffcc
</commit_message>
<xml_diff>
--- a/TEST_DEFINITIVO.xlsx
+++ b/TEST_DEFINITIVO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1092,8 +1092,6 @@
           <t>16</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>GOODWE ES UNIQ - GW8000-ES-C10 híbrido monofásico</t>
@@ -1114,7 +1112,6 @@
           <t>1</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr">
         <is>
           <t>Sí</t>
@@ -1123,6 +1120,64 @@
       <c r="N13" t="inlineStr">
         <is>
           <t>2025-09-25T07:50:43.054Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2663</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Juan Carlos 55</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Estructura coplanar NOVOTEGRA</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>MODULO FV JA SOLAR 535WP BLACK FRAME BIFACIAL 120 CELDAS</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>GOODWE GW6000-ES-20 híbrido monofásico</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>GOODWE Batería Lynx Home U G3 5,12 kWh</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>2025-06-25T13:59:26.816Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Crear/Actualizar Excel para pedido 68f8d57d82f06f0ab9ba552d
</commit_message>
<xml_diff>
--- a/TEST_DEFINITIVO.xlsx
+++ b/TEST_DEFINITIVO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1147,8 +1147,6 @@
           <t>12</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
           <t>GOODWE GW6000-ES-20 híbrido monofásico</t>
@@ -1169,7 +1167,6 @@
           <t>1</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr">
         <is>
           <t>Sí</t>
@@ -1178,6 +1175,64 @@
       <c r="N14" t="inlineStr">
         <is>
           <t>2025-06-25T13:59:26.816Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2060</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Angel Domenech Martin</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Estructura coplanar NOVOTEGRA</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>MODULO FV JA SOLAR 535WP BLACK FRAME BIFACIAL 120 CELDAS</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>GOODWE GW5000-ES-20 híbrido monofásico</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>GOODWE Batería Lynx Home U G3 5,12 kWh</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>2025-09-24T16:18:13.867Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Crear/Actualizar Excel para pedido 68c984b225de3a0af7c2e310
</commit_message>
<xml_diff>
--- a/TEST_DEFINITIVO.xlsx
+++ b/TEST_DEFINITIVO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1202,8 +1202,6 @@
           <t>10</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>GOODWE GW5000-ES-20 híbrido monofásico</t>
@@ -1224,7 +1222,6 @@
           <t>1</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
         <is>
           <t>Sí</t>
@@ -1233,6 +1230,56 @@
       <c r="N15" t="inlineStr">
         <is>
           <t>2025-09-24T16:18:13.867Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1598</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Juan José Lopez</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Estructura coplanar NOVOTEGRA</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Trina 505W TSM-NEG18R.25</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>GOODWE ES UNIQ - GW10000-ES-C10 híbrido monofásico</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>2024-01-03T10:49:29.088Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Crear/Actualizar Excel para pedido 68dfab4a8e9c4a0ab3cae911
</commit_message>
<xml_diff>
--- a/TEST_DEFINITIVO.xlsx
+++ b/TEST_DEFINITIVO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1257,8 +1257,6 @@
           <t>19</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>GOODWE ES UNIQ - GW10000-ES-C10 híbrido monofásico</t>
@@ -1269,9 +1267,6 @@
           <t>1</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr">
         <is>
           <t>Sí</t>
@@ -1280,6 +1275,64 @@
       <c r="N16" t="inlineStr">
         <is>
           <t>2024-01-03T10:49:29.088Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1827</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Jose luis Navarro</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Estructura coplanar NOVOTEGRA</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>MODULO FV JA SOLAR 535WP BLACK FRAME BIFACIAL 120 CELDAS</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>GOODWE ES UNIQ - GW10000-ES-C10 híbrido monofásico</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>GOODWE Batería Lynx Home U G3 5,12 kWh</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>2025-09-24T16:18:13.867Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Crear/Actualizar Excel para pedido 68f11532c36e740ad291764f
</commit_message>
<xml_diff>
--- a/TEST_DEFINITIVO.xlsx
+++ b/TEST_DEFINITIVO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1302,8 +1302,6 @@
           <t>20</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
           <t>GOODWE ES UNIQ - GW10000-ES-C10 híbrido monofásico</t>
@@ -1324,7 +1322,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr">
         <is>
           <t>Sí</t>
@@ -1333,6 +1330,56 @@
       <c r="N17" t="inlineStr">
         <is>
           <t>2025-09-24T16:18:13.867Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1971</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Ignacio Rodriguez</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Estructura coplanar NOVOTEGRA</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>MODULO FV JA SOLAR 535WP BLACK FRAME BIFACIAL 120 CELDAS</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>GOODWE GW3600-ES-20 híbrido monofásico</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>2025-09-25T07:50:43.054Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Crear/Actualizar Excel para pedido 69249e010f48bb0af0483b7d
</commit_message>
<xml_diff>
--- a/TEST_DEFINITIVO.xlsx
+++ b/TEST_DEFINITIVO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1357,8 +1357,6 @@
           <t>6</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
           <t>GOODWE GW3600-ES-20 híbrido monofásico</t>
@@ -1369,15 +1367,70 @@
           <t>1</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
           <t>Sí</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
+        <is>
+          <t>2025-09-25T07:50:43.054Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2804</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Marcos Cortecero Torres</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Estructura coplanar NOVOTEGRA</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>MODULO FV JA SOLAR 535WP BLACK FRAME BIFACIAL 120 CELDAS</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>GOODWE GW6000-ES-20 híbrido monofásico</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>GOODWE Batería Lynx Home U G3 5,12 kWh</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
         <is>
           <t>2025-09-25T07:50:43.054Z</t>
         </is>

</xml_diff>

<commit_message>
Crear/Actualizar Excel para pedido 691ee840d9cd7e0aaa545c84
</commit_message>
<xml_diff>
--- a/TEST_DEFINITIVO.xlsx
+++ b/TEST_DEFINITIVO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1402,8 +1402,6 @@
           <t>14</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
           <t>GOODWE GW6000-ES-20 híbrido monofásico</t>
@@ -1424,13 +1422,70 @@
           <t>1</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr">
         <is>
           <t>Sí</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
+        <is>
+          <t>2025-09-25T07:50:43.054Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2743</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Mayte López</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Estructura coplanar NOVOTEGRA</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>MODULO FV JA SOLAR 535WP BLACK FRAME BIFACIAL 120 CELDAS</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>GOODWE GW5000-ES-20 híbrido monofásico</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>GOODWE Batería Lynx Home U G3 5,12 kWh</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
         <is>
           <t>2025-09-25T07:50:43.054Z</t>
         </is>

</xml_diff>